<commit_message>
new changes in keyword driven fw
</commit_message>
<xml_diff>
--- a/KeywordDrivenHubspot.com/src/main/java/com/qa/hs/keyword/scenarios/hubspot_scenarios.xlsx
+++ b/KeywordDrivenHubspot.com/src/main/java/com/qa/hs/keyword/scenarios/hubspot_scenarios.xlsx
@@ -8,20 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="signup" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
   <si>
     <t>test step</t>
   </si>
   <si>
-    <t>locator</t>
-  </si>
-  <si>
     <t>action</t>
   </si>
   <si>
@@ -43,9 +41,6 @@
     <t>enter email address</t>
   </si>
   <si>
-    <t>id=username</t>
-  </si>
-  <si>
     <t>enter url</t>
   </si>
   <si>
@@ -61,15 +56,9 @@
     <t>enter password</t>
   </si>
   <si>
-    <t>id=password</t>
-  </si>
-  <si>
     <t>click on login button</t>
   </si>
   <si>
-    <t>id=loginBtn</t>
-  </si>
-  <si>
     <t>click</t>
   </si>
   <si>
@@ -85,7 +74,58 @@
     <t>Time@2020</t>
   </si>
   <si>
-    <t>linkText=Sign up</t>
+    <t>locatorValue</t>
+  </si>
+  <si>
+    <t>locatorType</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>loginBtn</t>
+  </si>
+  <si>
+    <t>Sign up</t>
+  </si>
+  <si>
+    <t>linkText</t>
+  </si>
+  <si>
+    <t>verify home page header</t>
+  </si>
+  <si>
+    <t>get Home Page Header text</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>isDisplayed</t>
+  </si>
+  <si>
+    <t>getText</t>
+  </si>
+  <si>
+    <t>Set up your HubSpot account</t>
+  </si>
+  <si>
+    <t>className</t>
+  </si>
+  <si>
+    <t>private-header__heading</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>//div//h1</t>
   </si>
 </sst>
 </file>
@@ -445,179 +485,288 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
+      <c r="E5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D5" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>